<commit_message>
sixth commit - add logout test case
</commit_message>
<xml_diff>
--- a/resources/DataProfileMenu.xlsx
+++ b/resources/DataProfileMenu.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romadonz/Documents/Zanuar/DANA/G2Lab/FinalProject/QuotaAppTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2BAF34-871D-5741-B84C-F86516292E9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F5C15C-8A0C-6041-BEAF-C1E45C5C3BFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" xr2:uid="{57623300-8E2D-C54C-A558-4EEA7A09C665}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="4" xr2:uid="{57623300-8E2D-C54C-A558-4EEA7A09C665}"/>
   </bookViews>
   <sheets>
     <sheet name="Change Full Name" sheetId="1" r:id="rId1"/>
     <sheet name="Change Email" sheetId="2" r:id="rId2"/>
     <sheet name="Change Phone Number" sheetId="6" r:id="rId3"/>
     <sheet name="Change Password" sheetId="4" r:id="rId4"/>
+    <sheet name="Logout" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="64">
   <si>
     <t>password</t>
   </si>
@@ -120,13 +121,121 @@
   </si>
   <si>
     <t>responsebody</t>
+  </si>
+  <si>
+    <t>phoneNumber</t>
+  </si>
+  <si>
+    <t>statusCodeRequest</t>
+  </si>
+  <si>
+    <t>responseBodyRequest</t>
+  </si>
+  <si>
+    <t>negative case - invalid phone number and password</t>
+  </si>
+  <si>
+    <t>not a number</t>
+  </si>
+  <si>
+    <t>012345678</t>
+  </si>
+  <si>
+    <t>negative case - invalid phone number</t>
+  </si>
+  <si>
+    <t>4bsurd d4t4</t>
+  </si>
+  <si>
+    <t>Zanuar30@@</t>
+  </si>
+  <si>
+    <t>negative case - invalid password</t>
+  </si>
+  <si>
+    <t>+6281252930398</t>
+  </si>
+  <si>
+    <t>401</t>
+  </si>
+  <si>
+    <t>Unauthorized</t>
+  </si>
+  <si>
+    <t>positif case - valid phone number and password</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>negative case - invalid phone number format (not numerical)</t>
+  </si>
+  <si>
+    <t>negative case - invalid phone number format (exceed 12 characters)</t>
+  </si>
+  <si>
+    <t>+628123456789101112</t>
+  </si>
+  <si>
+    <t>negative case - invalid phone number (outside Indonesia)</t>
+  </si>
+  <si>
+    <t>+601300808888</t>
+  </si>
+  <si>
+    <t>negative case - invalid phone number (unregistered number)</t>
+  </si>
+  <si>
+    <t>+6281234567890</t>
+  </si>
+  <si>
+    <t>negative case - invalid phone number (unverified number)</t>
+  </si>
+  <si>
+    <t>+6285785161197</t>
+  </si>
+  <si>
+    <t>negative case - invalid password (no lower case alphabetical character)</t>
+  </si>
+  <si>
+    <t>PASSWORD12345@@</t>
+  </si>
+  <si>
+    <t>negative case - invalid password (no upper case alphabetical character)</t>
+  </si>
+  <si>
+    <t>password12345@@</t>
+  </si>
+  <si>
+    <t>negative case - invalid password (no special character)</t>
+  </si>
+  <si>
+    <t>Password12345</t>
+  </si>
+  <si>
+    <t>negative case - invalid password (no numerical character)</t>
+  </si>
+  <si>
+    <t>PasswordSalah@@</t>
+  </si>
+  <si>
+    <t>negative case - invalid password (below 8 characters)</t>
+  </si>
+  <si>
+    <t>Pwd123@</t>
+  </si>
+  <si>
+    <t>negative case - invalid password (exceed 16 characters)</t>
+  </si>
+  <si>
+    <t>PasswordMelebihi16Karakter@@</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -140,8 +249,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -151,6 +267,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFD5967"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -182,12 +316,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,7 +659,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F9959BB-4BD4-1645-834F-8040D5B979C6}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -1306,4 +1461,298 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD92308A-CB7B-7B41-82FA-7A29955FA184}">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="61" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add edit user feature
</commit_message>
<xml_diff>
--- a/resources/DataProfileMenu.xlsx
+++ b/resources/DataProfileMenu.xlsx
@@ -8,16 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romadonz/Documents/Zanuar/DANA/G2Lab/FinalProject/QuotaAppTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D112ECF-19F6-944A-B8B2-46E7FB63760D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1317943D-4ACE-414E-A476-494E8296251E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" activeTab="4" xr2:uid="{57623300-8E2D-C54C-A558-4EEA7A09C665}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" activeTab="1" xr2:uid="{57623300-8E2D-C54C-A558-4EEA7A09C665}"/>
   </bookViews>
   <sheets>
-    <sheet name="Change Full Name" sheetId="1" r:id="rId1"/>
-    <sheet name="Change Email" sheetId="2" r:id="rId2"/>
-    <sheet name="Change Phone Number" sheetId="6" r:id="rId3"/>
-    <sheet name="Change Password" sheetId="4" r:id="rId4"/>
-    <sheet name="Logout" sheetId="8" r:id="rId5"/>
+    <sheet name="Edit User" sheetId="1" r:id="rId1"/>
+    <sheet name="Change Password" sheetId="4" r:id="rId2"/>
+    <sheet name="Logout" sheetId="8" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="59">
   <si>
     <t>password</t>
   </si>
@@ -63,9 +61,6 @@
     <t>fullname</t>
   </si>
   <si>
-    <t>email</t>
-  </si>
-  <si>
     <t>phonenumber</t>
   </si>
   <si>
@@ -105,12 +100,6 @@
     <t>timeout otp code</t>
   </si>
   <si>
-    <t>wrong email</t>
-  </si>
-  <si>
-    <t>blank email</t>
-  </si>
-  <si>
     <t>wrong new password</t>
   </si>
   <si>
@@ -138,13 +127,7 @@
     <t>not a number</t>
   </si>
   <si>
-    <t>012345678</t>
-  </si>
-  <si>
     <t>negative case - invalid phone number</t>
-  </si>
-  <si>
-    <t>4bsurd d4t4</t>
   </si>
   <si>
     <t>Zanuar30@@</t>
@@ -278,13 +261,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFD5967"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor rgb="FFFA827F"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -316,11 +299,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -331,8 +313,11 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -340,15 +325,18 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFA827F"/>
+      <color rgb="FFFD5967"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -660,7 +648,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -682,7 +670,7 @@
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -691,15 +679,15 @@
         <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -710,7 +698,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -732,7 +720,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -743,7 +731,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -754,7 +742,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -776,7 +764,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -787,7 +775,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -797,8 +785,8 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>18</v>
+      <c r="A11" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -808,8 +796,8 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>19</v>
+      <c r="A12" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -819,7 +807,7 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="2"/>
@@ -830,7 +818,7 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B14" s="2"/>
@@ -841,8 +829,8 @@
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>20</v>
+      <c r="A15" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -852,8 +840,8 @@
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>21</v>
+      <c r="A16" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -869,394 +857,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7189700-26BE-B342-926E-EF81568121D9}">
-  <dimension ref="A1:H16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" s="3"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED8D8A7E-F8A4-4F41-BE15-873B0010E036}">
-  <dimension ref="A1:F14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{865360DB-CC0A-7D49-8F52-9B29FD828225}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1275,27 +880,27 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1306,7 +911,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1328,7 +933,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -1339,7 +944,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1350,7 +955,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1372,7 +977,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1383,7 +988,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1393,8 +998,8 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>18</v>
+      <c r="A11" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1404,8 +1009,8 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>19</v>
+      <c r="A12" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1415,7 +1020,7 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="2"/>
@@ -1426,7 +1031,7 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B14" s="2"/>
@@ -1437,8 +1042,8 @@
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>20</v>
+      <c r="A15" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1448,8 +1053,8 @@
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>21</v>
+      <c r="A16" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1463,12 +1068,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD92308A-CB7B-7B41-82FA-7A29955FA184}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1481,275 +1086,275 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="B2" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="C2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="B3" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="D3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="C4" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="B8" s="9" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="C8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="E8" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="9" t="s">
+      <c r="B9" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+      <c r="C9" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+      <c r="B10" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="C10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+      <c r="B11" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="D11" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+      <c r="B12" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="D12" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
+      <c r="B13" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="7" t="s">
+      <c r="D13" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="11" t="s">
+      <c r="B14" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="7" t="s">
+      <c r="D14" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="11" t="s">
+      <c r="B15" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="7" t="s">
+      <c r="D15" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="11" t="s">
+      <c r="B16" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>40</v>
+      <c r="D16" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>